<commit_message>
ADAPT ates.py, ttes.py and ites.py
</commit_message>
<xml_diff>
--- a/results/[0_basic]_#_fix_cost.xlsx
+++ b/results/[0_basic]_#_fix_cost.xlsx
@@ -492,10 +492,10 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>1082.89975647011</v>
+        <v>1082.899756470087</v>
       </c>
       <c r="B2" t="n">
-        <v>488.4827730520537</v>
+        <v>488.482773052096</v>
       </c>
       <c r="C2" t="n">
         <v>0</v>
@@ -510,7 +510,7 @@
         <v>0</v>
       </c>
       <c r="G2" t="n">
-        <v>8095.925712661734</v>
+        <v>8095.925712661834</v>
       </c>
       <c r="H2" t="n">
         <v>0</v>
@@ -519,7 +519,7 @@
         <v>0</v>
       </c>
       <c r="J2" t="n">
-        <v>5820.297176149042</v>
+        <v>5820.297176149008</v>
       </c>
     </row>
   </sheetData>
@@ -595,10 +595,10 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>5855.63995427043</v>
+        <v>5855.639954270414</v>
       </c>
       <c r="B2" t="n">
-        <v>488.4827730520537</v>
+        <v>488.482773052096</v>
       </c>
       <c r="C2" t="n">
         <v>0</v>
@@ -607,13 +607,13 @@
         <v>0</v>
       </c>
       <c r="E2" t="n">
-        <v>41137.20798023105</v>
+        <v>41137.20798023103</v>
       </c>
       <c r="F2" t="n">
         <v>0</v>
       </c>
       <c r="G2" t="n">
-        <v>8095.925712661734</v>
+        <v>8095.925712661834</v>
       </c>
       <c r="H2" t="n">
         <v>0</v>
@@ -622,7 +622,7 @@
         <v>0</v>
       </c>
       <c r="J2" t="n">
-        <v>18566.05691013583</v>
+        <v>18566.05691013579</v>
       </c>
     </row>
   </sheetData>
@@ -698,10 +698,10 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>11110.86551379928</v>
+        <v>11110.86551379931</v>
       </c>
       <c r="B2" t="n">
-        <v>488.4827730520537</v>
+        <v>488.482773052096</v>
       </c>
       <c r="C2" t="n">
         <v>0</v>
@@ -710,13 +710,13 @@
         <v>0</v>
       </c>
       <c r="E2" t="n">
-        <v>101297.3375424221</v>
+        <v>101297.3375424222</v>
       </c>
       <c r="F2" t="n">
         <v>0</v>
       </c>
       <c r="G2" t="n">
-        <v>8095.925712661734</v>
+        <v>8095.925712661834</v>
       </c>
       <c r="H2" t="n">
         <v>0</v>
@@ -725,7 +725,7 @@
         <v>0</v>
       </c>
       <c r="J2" t="n">
-        <v>28353.5264413284</v>
+        <v>28353.52644132823</v>
       </c>
     </row>
   </sheetData>
@@ -801,10 +801,10 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>11110.86551379928</v>
+        <v>11110.86551379931</v>
       </c>
       <c r="B2" t="n">
-        <v>488.4827730520537</v>
+        <v>488.482773052096</v>
       </c>
       <c r="C2" t="n">
         <v>0</v>
@@ -813,13 +813,13 @@
         <v>0</v>
       </c>
       <c r="E2" t="n">
-        <v>101297.3375424221</v>
+        <v>101297.3375424222</v>
       </c>
       <c r="F2" t="n">
         <v>0</v>
       </c>
       <c r="G2" t="n">
-        <v>8095.925712661734</v>
+        <v>8095.925712661834</v>
       </c>
       <c r="H2" t="n">
         <v>0</v>
@@ -828,7 +828,7 @@
         <v>0</v>
       </c>
       <c r="J2" t="n">
-        <v>28353.5264413284</v>
+        <v>28353.52644132823</v>
       </c>
     </row>
   </sheetData>
@@ -904,10 +904,10 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>11110.86551379928</v>
+        <v>11110.86551379931</v>
       </c>
       <c r="B2" t="n">
-        <v>488.4827730520537</v>
+        <v>488.482773052096</v>
       </c>
       <c r="C2" t="n">
         <v>0</v>
@@ -916,13 +916,13 @@
         <v>0</v>
       </c>
       <c r="E2" t="n">
-        <v>101297.3375424221</v>
+        <v>101297.3375424222</v>
       </c>
       <c r="F2" t="n">
         <v>0</v>
       </c>
       <c r="G2" t="n">
-        <v>8095.925712661734</v>
+        <v>8095.925712661834</v>
       </c>
       <c r="H2" t="n">
         <v>0</v>
@@ -931,7 +931,7 @@
         <v>0</v>
       </c>
       <c r="J2" t="n">
-        <v>28353.5264413284</v>
+        <v>28353.52644132823</v>
       </c>
     </row>
   </sheetData>
@@ -1007,10 +1007,10 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>11110.86551379928</v>
+        <v>11110.86551379931</v>
       </c>
       <c r="B2" t="n">
-        <v>488.4827730520537</v>
+        <v>488.482773052096</v>
       </c>
       <c r="C2" t="n">
         <v>0</v>
@@ -1019,13 +1019,13 @@
         <v>0</v>
       </c>
       <c r="E2" t="n">
-        <v>101297.3375424221</v>
+        <v>101297.3375424222</v>
       </c>
       <c r="F2" t="n">
         <v>0</v>
       </c>
       <c r="G2" t="n">
-        <v>8095.925712661734</v>
+        <v>8095.925712661834</v>
       </c>
       <c r="H2" t="n">
         <v>0</v>
@@ -1034,7 +1034,7 @@
         <v>0</v>
       </c>
       <c r="J2" t="n">
-        <v>28353.5264413284</v>
+        <v>28353.52644132823</v>
       </c>
     </row>
   </sheetData>

</xml_diff>